<commit_message>
added Kat's r script, tutorial heatmap data
</commit_message>
<xml_diff>
--- a/nph13389-sup-0002-TableS1.xlsx
+++ b/nph13389-sup-0002-TableS1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24720" windowHeight="15600" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Male vs Female" sheetId="1" r:id="rId1"/>
@@ -7754,7 +7754,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M276"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="E4" sqref="E4"/>
     </sheetView>
@@ -39707,7 +39707,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="5" topLeftCell="A37" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C54" sqref="C54"/>
     </sheetView>

</xml_diff>

<commit_message>
added to presentation, normalized in R script too DM
</commit_message>
<xml_diff>
--- a/nph13389-sup-0002-TableS1.xlsx
+++ b/nph13389-sup-0002-TableS1.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17329"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Devin\Documents\GradSchool\IowaState\EEOB_546X\BCB546X-Spring2017_Valerin_final_project\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760" tabRatio="500"/>
   </bookViews>
@@ -7278,7 +7283,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -7425,6 +7430,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -7755,7 +7763,7 @@
   <dimension ref="A1:M276"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="5" topLeftCell="A270" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
@@ -18753,7 +18761,7 @@
   <dimension ref="A1:M488"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="5" topLeftCell="A477" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
@@ -38228,7 +38236,7 @@
   <dimension ref="A1:M40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="5" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>

</xml_diff>